<commit_message>
updated data file with cases up to 14 days prior
</commit_message>
<xml_diff>
--- a/data_dictionary_covid_cases_restricted_detailed.xlsx
+++ b/data_dictionary_covid_cases_restricted_detailed.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{DF368E8A-F4D9-4DD5-A040-6D30471ABBC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DAE807-644A-A848-A3F6-CE835B0A644D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{3A1DE3AA-CD8F-48E4-8503-F6FD448E3099}"/>
+    <workbookView xWindow="9240" yWindow="1720" windowWidth="27740" windowHeight="18020" xr2:uid="{3A1DE3AA-CD8F-48E4-8503-F6FD448E3099}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>MM/DD/YYYY</t>
-  </si>
-  <si>
     <t>Age group</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>Last updated: May 3, 2020</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
   </si>
 </sst>
 </file>
@@ -688,28 +688,28 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.5" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="41.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="35" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="8" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -726,10 +726,10 @@
         <v>23</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -740,15 +740,15 @@
         <v>24</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>10</v>
@@ -757,17 +757,17 @@
         <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -784,9 +784,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>14</v>
@@ -795,47 +795,47 @@
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="B7" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>6</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>27</v>
+      <c r="D9" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>26</v>
@@ -861,7 +861,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -871,14 +871,14 @@
       <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>27</v>
+      <c r="D10" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -895,7 +895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
@@ -912,7 +912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
@@ -929,13 +929,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="C14" s="8" t="s">
         <v>24</v>
       </c>
@@ -946,12 +946,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>24</v>
@@ -965,12 +965,12 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>24</v>
@@ -984,12 +984,12 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>24</v>
@@ -1003,12 +1003,12 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>24</v>
@@ -1022,12 +1022,12 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>24</v>
@@ -1041,12 +1041,12 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>24</v>
@@ -1060,12 +1060,12 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>24</v>
@@ -1079,12 +1079,12 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>24</v>
@@ -1098,12 +1098,12 @@
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>24</v>
@@ -1117,12 +1117,12 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>24</v>
@@ -1136,12 +1136,12 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>24</v>
@@ -1155,12 +1155,12 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>24</v>
@@ -1174,12 +1174,12 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>24</v>
@@ -1193,12 +1193,12 @@
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>24</v>
@@ -1212,12 +1212,12 @@
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
     </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>24</v>
@@ -1231,12 +1231,12 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>24</v>
@@ -1250,7 +1250,7 @@
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Uploaded the most recent data dictionary
</commit_message>
<xml_diff>
--- a/data_dictionary_covid_cases_restricted_detailed.xlsx
+++ b/data_dictionary_covid_cases_restricted_detailed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23516"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA61FF-7984-4050-ACFC-702C13F31658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F106F01-4B7C-4EDF-ACCF-252DAC80AFD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A1DE3AA-CD8F-48E4-8503-F6FD448E3099}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,6 +21,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
   <si>
-    <t>Last updated: September 14, 2020</t>
+    <t>Last updated: November 19, 2020</t>
   </si>
   <si>
     <t>Description</t>
@@ -82,7 +83,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>This date was populated using the date at which a case record was first submitted to the database. If missing, then the report date entered on the case report form was used. If missing, then the date at which the case first appeared in the databse was used.</t>
+    <t>This date was populated using the date at which a case record was first submitted to the database. If missing, then the report date entered on the case report form was used. If missing, then the date at which the case first appeared in the database was used.</t>
   </si>
   <si>
     <t>Sex</t>
@@ -166,7 +167,7 @@
     <t>onset_dt</t>
   </si>
   <si>
-    <t>Date of first positive specimen collection (MM/DD/YYYY)</t>
+    <t>Date of first positive specimen collection</t>
   </si>
   <si>
     <t>pos_spec_dt</t>
@@ -307,7 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,27 +710,27 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="59.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="42.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="41.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="35" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="6"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="34.5" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -749,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="28.9">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -766,7 +767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="128.25" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
@@ -787,7 +788,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="57.6">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
@@ -804,7 +805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="7" customFormat="1" ht="149.25" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -824,7 +825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="129.6">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
@@ -844,7 +845,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="57.6">
       <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
@@ -862,7 +863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="7" customFormat="1">
       <c r="A9" s="12" t="s">
         <v>33</v>
       </c>
@@ -878,7 +879,7 @@
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="7" customFormat="1">
       <c r="A10" s="12" t="s">
         <v>35</v>
       </c>
@@ -894,7 +895,7 @@
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="1" customFormat="1">
       <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
@@ -913,7 +914,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="7" customFormat="1" ht="33" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
@@ -930,7 +931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="43.15">
       <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
@@ -947,7 +948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="7" customFormat="1" ht="43.15">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -964,7 +965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="43.15">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -981,7 +982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="7" customFormat="1" ht="43.15">
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
@@ -998,7 +999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="43.15">
       <c r="A17" s="8" t="s">
         <v>50</v>
       </c>
@@ -1017,7 +1018,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="43.15">
       <c r="A18" s="7" t="s">
         <v>52</v>
       </c>
@@ -1036,7 +1037,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="43.15">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -1055,7 +1056,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="43.15">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1074,7 +1075,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A21" s="8" t="s">
         <v>58</v>
       </c>
@@ -1093,7 +1094,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -1112,7 +1113,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A23" s="8" t="s">
         <v>62</v>
       </c>
@@ -1131,7 +1132,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A24" s="8" t="s">
         <v>64</v>
       </c>
@@ -1150,7 +1151,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A25" s="8" t="s">
         <v>66</v>
       </c>
@@ -1169,7 +1170,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A26" s="8" t="s">
         <v>68</v>
       </c>
@@ -1188,7 +1189,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A27" s="8" t="s">
         <v>70</v>
       </c>
@@ -1207,7 +1208,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A28" s="8" t="s">
         <v>72</v>
       </c>
@@ -1226,7 +1227,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A29" s="8" t="s">
         <v>74</v>
       </c>
@@ -1245,7 +1246,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A30" s="8" t="s">
         <v>76</v>
       </c>
@@ -1264,7 +1265,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A31" s="8" t="s">
         <v>78</v>
       </c>
@@ -1283,7 +1284,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="43.15">
       <c r="A32" s="8" t="s">
         <v>80</v>
       </c>
@@ -1302,7 +1303,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="7" customFormat="1" ht="43.15">
       <c r="A33" s="8" t="s">
         <v>82</v>
       </c>
@@ -1554,47 +1555,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4D23129-BA43-4A2F-A94A-EB23F1BAD1F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4D23129-BA43-4A2F-A94A-EB23F1BAD1F0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BA1AD85-4B7C-4300-BEFB-DCB090DF7E12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="a12d8773-0f30-405c-b193-40869fe1c1e6"/>
-    <ds:schemaRef ds:uri="1edd9f51-35c2-425f-bf6f-7b72bac0b145"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BA1AD85-4B7C-4300-BEFB-DCB090DF7E12}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6929926F-7FAB-4221-93CC-ED28560DD47F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1edd9f51-35c2-425f-bf6f-7b72bac0b145"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="a12d8773-0f30-405c-b193-40869fe1c1e6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6929926F-7FAB-4221-93CC-ED28560DD47F}"/>
 </file>
</xml_diff>

<commit_message>
December update of restricted detailed data set
</commit_message>
<xml_diff>
--- a/data_dictionary_covid_cases_restricted_detailed.xlsx
+++ b/data_dictionary_covid_cases_restricted_detailed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F106F01-4B7C-4EDF-ACCF-252DAC80AFD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B65846-4435-4E9E-A621-44ED10490A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A1DE3AA-CD8F-48E4-8503-F6FD448E3099}"/>
+    <workbookView xWindow="1416" yWindow="600" windowWidth="21624" windowHeight="12360" xr2:uid="{3A1DE3AA-CD8F-48E4-8503-F6FD448E3099}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,9 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
-  <si>
-    <t>Last updated: November 19, 2020</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
+  <si>
+    <t>Last updated: December 21, 2020</t>
   </si>
   <si>
     <t>Description</t>
@@ -84,6 +83,12 @@
   </si>
   <si>
     <t>This date was populated using the date at which a case record was first submitted to the database. If missing, then the report date entered on the case report form was used. If missing, then the date at which the case first appeared in the database was used.</t>
+  </si>
+  <si>
+    <t>The earlier of the Clinical Date (date related to the illness or specimen collection) or the Date Received by CDC</t>
+  </si>
+  <si>
+    <t>Cdc_case_earliest_dt uses the best available date from both cdc_received_dt and cdc_clinical_obs_dt and is an option to end-users who need a date variable with optimized completeness. The logic of cdc_case_earliest_dt is to use the non-null date of one variable when the other is null and to use the earliest valid date when both dates are available.</t>
   </si>
   <si>
     <t>Sex</t>
@@ -303,12 +308,15 @@
   <si>
     <t>medcond_yn</t>
   </si>
+  <si>
+    <t>cdc_case_earliest_dt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +343,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -356,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -391,6 +406,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,31 +727,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC5408C-34B2-4BD5-B368-D579A8A3CC4C}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" style="6" customWidth="1"/>
     <col min="7" max="7" width="35" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="34.5" customHeight="1">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -750,7 +771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="28.9">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -767,7 +788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="128.25" customHeight="1">
+    <row r="4" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
@@ -788,98 +809,103 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="57.6">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" ht="149.25" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" ht="129.6">
-      <c r="A7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="57.6">
-      <c r="A8" s="14" t="s">
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="E8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="14" t="s">
+    </row>
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="7" customFormat="1">
-      <c r="A9" s="12" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="F9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" s="7" customFormat="1">
+    </row>
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>35</v>
       </c>
@@ -895,33 +921,30 @@
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" ht="33" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -930,42 +953,44 @@
       <c r="E12" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="43.15">
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" ht="43.15">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="43.15">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -976,13 +1001,13 @@
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="43.15">
+    <row r="16" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
@@ -993,14 +1018,14 @@
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="43.15">
-      <c r="A17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1010,16 +1035,14 @@
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="43.15">
-      <c r="A18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1029,15 +1052,15 @@
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="43.15">
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -1048,15 +1071,15 @@
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="43.15">
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1067,34 +1090,34 @@
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="43.15">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:7" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="43.15">
+        <v>45</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -1105,7 +1128,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>11</v>
@@ -1113,7 +1136,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>62</v>
       </c>
@@ -1124,7 +1147,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>11</v>
@@ -1132,7 +1155,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>64</v>
       </c>
@@ -1143,7 +1166,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>11</v>
@@ -1151,7 +1174,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>66</v>
       </c>
@@ -1162,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>11</v>
@@ -1170,7 +1193,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>68</v>
       </c>
@@ -1181,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>11</v>
@@ -1189,7 +1212,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>70</v>
       </c>
@@ -1200,7 +1223,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>11</v>
@@ -1208,7 +1231,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>72</v>
       </c>
@@ -1219,7 +1242,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>11</v>
@@ -1227,7 +1250,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="29" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>74</v>
       </c>
@@ -1238,7 +1261,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>11</v>
@@ -1246,7 +1269,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>76</v>
       </c>
@@ -1257,7 +1280,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>11</v>
@@ -1265,7 +1288,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="31" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>78</v>
       </c>
@@ -1276,7 +1299,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>11</v>
@@ -1284,7 +1307,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" ht="43.15">
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>80</v>
       </c>
@@ -1295,7 +1318,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>11</v>
@@ -1303,7 +1326,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="43.15">
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>82</v>
       </c>
@@ -1314,9 +1337,28 @@
         <v>9</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1336,6 +1378,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100421E03D7E06C234EB5626DEC4B2F4B58" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d681b795e1ce027f209e0641691074eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="a12d8773-0f30-405c-b193-40869fe1c1e6" xmlns:ns3="1edd9f51-35c2-425f-bf6f-7b72bac0b145" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09d6ed279c48a47a29cd1cd984c3b420" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1545,23 +1596,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4D23129-BA43-4A2F-A94A-EB23F1BAD1F0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4D23129-BA43-4A2F-A94A-EB23F1BAD1F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BA1AD85-4B7C-4300-BEFB-DCB090DF7E12}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6929926F-7FAB-4221-93CC-ED28560DD47F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6929926F-7FAB-4221-93CC-ED28560DD47F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BA1AD85-4B7C-4300-BEFB-DCB090DF7E12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="a12d8773-0f30-405c-b193-40869fe1c1e6"/>
+    <ds:schemaRef ds:uri="1edd9f51-35c2-425f-bf6f-7b72bac0b145"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>